<commit_message>
feat: can now add products to db
</commit_message>
<xml_diff>
--- a/excel-data/Sneakers-data.xlsx
+++ b/excel-data/Sneakers-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan.joe.haboc\Desktop\Polder\the_odin_project\shop-app\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FE259D9-52D8-48BF-A742-0390A8ABA148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E300ACF7-EFF4-49DF-B828-0DDB0EF907EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2617201D-6CC6-47DF-B8AD-9E26E53B1F66}"/>
   </bookViews>
@@ -48,9 +48,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
-    <t>Column1.price</t>
-  </si>
-  <si>
     <t>Adidas NMD</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Sneakers</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
     <tableColumn id="1" xr3:uid="{2B4D4A82-6246-49A8-B6FF-54AB4CC9213F}" uniqueName="1" name="title" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{CECA7BC3-A18C-415C-BD80-1D587590AA1E}" uniqueName="2" name="name" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D72D1C3F-95CA-401A-81F4-31172651F467}" uniqueName="3" name="imageUrl" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{6B6AA2E5-29E8-4D15-8A8C-AD8CE221182E}" uniqueName="4" name="Column1.price" queryTableFieldId="4"/>
+    <tableColumn id="4" xr3:uid="{6B6AA2E5-29E8-4D15-8A8C-AD8CE221182E}" uniqueName="4" name="price" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,27 +502,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
       <c r="D2">
         <v>220</v>
@@ -530,13 +530,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
       <c r="D3">
         <v>280</v>
@@ -544,13 +544,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
       <c r="D4">
         <v>110</v>
@@ -558,13 +558,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
       <c r="D5">
         <v>160</v>
@@ -572,13 +572,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
       <c r="D6">
         <v>160</v>
@@ -586,13 +586,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
       <c r="D7">
         <v>160</v>
@@ -600,13 +600,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
       <c r="D8">
         <v>190</v>
@@ -614,13 +614,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9">
         <v>200</v>

</xml_diff>